<commit_message>
Started working on Read-in of region selection
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Documents\git\GENeSYS-MOD_GroupRepo\GENeSYS-MOD_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE09A2D-8EC6-4C49-8EE5-E7E0F115D3E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA26F5F-E08B-44B6-B009-EA58A77FB28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>Continent</t>
   </si>
@@ -75,15 +75,6 @@
   </si>
   <si>
     <t>Region Selected</t>
-  </si>
-  <si>
-    <t>Country-Node</t>
-  </si>
-  <si>
-    <t>Country_Sublevel_1_Node</t>
-  </si>
-  <si>
-    <t>Country_Sublevel_2_Node</t>
   </si>
 </sst>
 </file>
@@ -123,7 +114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +130,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,18 +426,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:J17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,17 +453,8 @@
       <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -488,17 +470,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -514,17 +487,8 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -540,17 +504,8 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -564,10 +519,10 @@
         <v>8</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -584,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -598,10 +553,10 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -615,10 +570,10 @@
         <v>12</v>
       </c>
       <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -635,7 +590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -665,7 +620,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -677,7 +632,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User input settings update
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Documents\git\GENeSYS-MOD_GroupRepo\GENeSYS-MOD_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA26F5F-E08B-44B6-B009-EA58A77FB28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66AC37F-BD48-407F-8A48-0151A04ED2CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="44">
   <si>
     <t>Continent</t>
   </si>
@@ -75,6 +75,90 @@
   </si>
   <si>
     <t>Region Selected</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>NONEU_Balkan</t>
   </si>
 </sst>
 </file>
@@ -110,11 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -130,7 +215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,13 +511,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -605,6 +690,516 @@
       </c>
       <c r="E10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -620,7 +1215,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -632,7 +1227,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update user input settings file - country codes for europe added
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA26F5F-E08B-44B6-B009-EA58A77FB28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7509A4-5545-463E-BD73-644F39DEEAE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="44">
   <si>
     <t>Continent</t>
   </si>
@@ -75,6 +75,90 @@
   </si>
   <si>
     <t>Region Selected</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>NONEU_Balkan</t>
   </si>
 </sst>
 </file>
@@ -110,11 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -130,7 +215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,13 +511,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -604,6 +689,516 @@
         <v>14</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40">
         <v>1</v>
       </c>
     </row>
@@ -620,7 +1215,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -632,7 +1227,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Script reads csvs, creates excel
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dozeumhep\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7509A4-5545-463E-BD73-644F39DEEAE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20227B78-0085-4342-8073-84A3261E06F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -194,12 +194,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -215,7 +214,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -514,10 +513,10 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -696,13 +695,13 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11">
@@ -713,13 +712,13 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
       <c r="E12">
@@ -730,13 +729,13 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>18</v>
       </c>
       <c r="E13">
@@ -747,13 +746,13 @@
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14">
@@ -764,13 +763,13 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="E15">
@@ -781,30 +780,30 @@
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>21</v>
       </c>
       <c r="E17">
@@ -815,13 +814,13 @@
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18">
@@ -832,13 +831,13 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>23</v>
       </c>
       <c r="E19">
@@ -849,13 +848,13 @@
       <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>24</v>
       </c>
       <c r="E20">
@@ -866,13 +865,13 @@
       <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>25</v>
       </c>
       <c r="E21">
@@ -883,13 +882,13 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>26</v>
       </c>
       <c r="E22">
@@ -900,13 +899,13 @@
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>27</v>
       </c>
       <c r="E23">
@@ -917,13 +916,13 @@
       <c r="A24" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>28</v>
       </c>
       <c r="E24">
@@ -934,13 +933,13 @@
       <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
       <c r="E25">
@@ -951,13 +950,13 @@
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>30</v>
       </c>
       <c r="E26">
@@ -968,13 +967,13 @@
       <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>31</v>
       </c>
       <c r="E27">
@@ -985,13 +984,13 @@
       <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>32</v>
       </c>
       <c r="E28">
@@ -1002,13 +1001,13 @@
       <c r="A29" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>33</v>
       </c>
       <c r="E29">
@@ -1019,13 +1018,13 @@
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>34</v>
       </c>
       <c r="E30">
@@ -1036,13 +1035,13 @@
       <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31">
@@ -1053,13 +1052,13 @@
       <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>35</v>
       </c>
       <c r="E32">
@@ -1070,13 +1069,13 @@
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>36</v>
       </c>
       <c r="E33">
@@ -1087,13 +1086,13 @@
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>37</v>
       </c>
       <c r="E34">
@@ -1104,13 +1103,13 @@
       <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>38</v>
       </c>
       <c r="E35">
@@ -1121,13 +1120,13 @@
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>39</v>
       </c>
       <c r="E36">
@@ -1138,13 +1137,13 @@
       <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>40</v>
       </c>
       <c r="E37">
@@ -1155,13 +1154,13 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>41</v>
       </c>
       <c r="E38">
@@ -1172,13 +1171,13 @@
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>42</v>
       </c>
       <c r="E39">
@@ -1189,13 +1188,13 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>43</v>
       </c>
       <c r="E40">
@@ -1215,7 +1214,7 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1227,7 +1226,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Include functionality to also filter for technology
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20227B78-0085-4342-8073-84A3261E06F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F0310F-B419-49DA-BA2B-A10EF33BDD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="49">
   <si>
     <t>Continent</t>
   </si>
@@ -159,6 +170,21 @@
   </si>
   <si>
     <t>NONEU_Balkan</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Technology Selected</t>
+  </si>
+  <si>
+    <t>Solar_PV</t>
+  </si>
+  <si>
+    <t>P_Gas</t>
+  </si>
+  <si>
+    <t>HLR_Biomass</t>
   </si>
 </sst>
 </file>
@@ -512,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -1208,14 +1234,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Years work now as well
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v01_phe_05-09-2023.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F0310F-B419-49DA-BA2B-A10EF33BDD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025897A9-7D3C-49F7-A31C-4EBC542AE81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="31500" yWindow="2700" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
     <sheet name="Technology_selection" sheetId="2" r:id="rId2"/>
-    <sheet name="Technology_in_region_selection" sheetId="3" r:id="rId3"/>
+    <sheet name="Year_selection" sheetId="4" r:id="rId3"/>
+    <sheet name="Technology_in_region_selection" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="51">
   <si>
     <t>Continent</t>
   </si>
@@ -185,6 +186,12 @@
   </si>
   <si>
     <t>HLR_Biomass</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Year selection</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1280,6 +1287,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386A4F90-CDC6-4413-A001-2349025B492F}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2030</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2035</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2040</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2045</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2050</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64D1206-FE0C-4D30-B550-10017D0BE07E}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>